<commit_message>
fixed grading added prob
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/Topic 2 Extra DQ 5.xlsx
+++ b/144F20/Topic 2/Topic 2 Extra DQ 5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5F8A7B-AC3A-4DB1-8785-68D195D96950}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{AEAE6585-0D7C-4162-A89E-07796AB4C7DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1308" yWindow="900" windowWidth="20796" windowHeight="11424" xr2:uid="{AF244846-4AAD-42AC-8F96-96B174BB4566}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="60">
   <si>
     <t>Quantity of</t>
   </si>
@@ -255,6 +255,47 @@
   <si>
     <t>lb/kg</t>
   </si>
+  <si>
+    <t>oz/ft^2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Convert ounces per square ft to grams per square meter</t>
+    </r>
+  </si>
+  <si>
+    <t>g/oz</t>
+  </si>
+  <si>
+    <t>g/m^2</t>
+  </si>
+  <si>
+    <t>Only the final answers are self grading.</t>
+  </si>
+  <si>
+    <t>Use entries from the conversion table to perform the following conversions.  Note that you may use entries only from the table above, even if a more direct conversion is possible.  For each part, the number of ratios required is shown in the table.  Note that your ratios for the formulas may be either one of the conversion factors above or the reciprocal, as illustrated in the example.  No special formatting is required for the cells containing your formulas.  In the blue cells, enter the ratio of units that you multiplied by for each conversion. You should use the abbreviations provided above, including capitalization as given.</t>
+  </si>
+  <si>
+    <t>ft/m</t>
+  </si>
 </sst>
 </file>
 
@@ -263,7 +304,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +315,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -318,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -637,11 +685,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -737,6 +964,70 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -745,86 +1036,109 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -837,13 +1151,6 @@
         <b/>
         <i val="0"/>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
       </font>
     </dxf>
   </dxfs>
@@ -861,99 +1168,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>869950</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C70DCE4-AD77-453F-9B33-87D57102ADAA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12700" y="5067300"/>
-          <a:ext cx="8420100" cy="1168400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Use entries from the conversion table to perform the following conversions.  Note that you may</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>use entries only from</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> the table above, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>even if a more direct conversion is possible.  For</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> each part, the number of ratios required is shown in the table.  Note that your ratios for the formulas may be either one of the conversion factors above or the reciprocal, as illustrated in the example.  No special formatting is required for the cells containing your formulas.  In the blue cells, enter the ratio of units that you multiplied by for each conversion. You should use the abbreviations provided above, including capitalization as given.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1234,8 +1448,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{642B9D2E-63F2-4FA0-915E-25855D920A90}">
-  <header guid="{642B9D2E-63F2-4FA0-915E-25855D920A90}" dateTime="2020-09-26T00:13:53" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A58227E2-4D60-41C5-91E7-BEC5E59B14DC}">
+  <header guid="{A58227E2-4D60-41C5-91E7-BEC5E59B14DC}" dateTime="2020-10-04T22:23:02" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1249,7 +1463,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{A58227E2-4D60-41C5-91E7-BEC5E59B14DC}" name="Richard Ketchersid" id="-1739560314" dateTime="2020-10-04T22:23:02"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1549,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE0E753-5E77-4073-B8CA-0383615E5C44}">
-  <dimension ref="A11:K39"/>
+  <dimension ref="A11:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,10 +1823,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1865,7 +2081,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1878,67 +2094,69 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+    <row r="24" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="62"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="65"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="A27" s="63"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="65"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="66"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1956,20 +2174,24 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="31" t="s">
+      <c r="C30" s="44"/>
+      <c r="D30" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="31" t="s">
+      <c r="E30" s="44"/>
+      <c r="F30" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="52"/>
     </row>
     <row r="31" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
@@ -1993,25 +2215,35 @@
       <c r="G31" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="H31" s="46">
+        <v>13</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="28"/>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="32" t="s">
         <v>35</v>
       </c>
       <c r="E32" s="30"/>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="32" t="s">
         <v>35</v>
       </c>
       <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H32" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="53"/>
+    </row>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>36</v>
       </c>
@@ -2025,25 +2257,31 @@
       <c r="E33" s="18"/>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="17"/>
+      <c r="I33" s="49"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="32" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="30"/>
-      <c r="F34" s="29" t="s">
+      <c r="F34" s="32" t="s">
         <v>35</v>
       </c>
       <c r="G34" s="30"/>
-    </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H34" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="53"/>
+    </row>
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>38</v>
       </c>
@@ -2057,49 +2295,61 @@
       <c r="E35" s="18"/>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="17"/>
+      <c r="I35" s="49"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="29" t="s">
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="32" t="s">
         <v>35</v>
       </c>
       <c r="G36" s="30"/>
-    </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H36" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="53"/>
+    </row>
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="17"/>
+      <c r="I37" s="49"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="29" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="30"/>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="29" t="s">
         <v>2</v>
       </c>
       <c r="G38" s="30"/>
-    </row>
-    <row r="39" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="53"/>
+    </row>
+    <row r="39" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
         <v>41</v>
       </c>
@@ -2113,17 +2363,46 @@
       <c r="E39" s="24"/>
       <c r="F39" s="23"/>
       <c r="G39" s="24"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="50"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E41" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="55"/>
+      <c r="G41" s="56"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E42" s="57"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="59"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Rwe46gXXBz7vaUBqmP98OwR3vbZNmi/B1kvZiPl244e9ueZCrOWphgBiE7aMhiV9+NmFOujrQ5ImW4QYgQAV/Q==" saltValue="ys5i917SCb4R9jblRcdXGw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jgC7epeQR5FjcDaoRFto27F3pz+rBPFgcxhFFExJo+xxdQwKkNOUf4DEFIiY0MmsCKKr2quyLlmcFQUR3CasNg==" saltValue="sgq4F9OGVvMvF+dPiEOCNw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <customSheetViews>
-    <customSheetView guid="{D3B99D0F-5290-4C19-9294-325A292E8E9A}" topLeftCell="A25">
-      <selection activeCell="C35" sqref="C35"/>
+    <customSheetView guid="{D3B99D0F-5290-4C19-9294-325A292E8E9A}" topLeftCell="A26">
+      <selection activeCell="F33" sqref="F33:G33"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="16">
+  <mergeCells count="23">
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="A24:H28"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:G38"/>
@@ -2133,13 +2412,6 @@
     <mergeCell ref="B36:C37"/>
     <mergeCell ref="D36:E37"/>
     <mergeCell ref="F36:G36"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="F30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2148,8 +2420,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{1096F20E-5F85-4D62-86B5-ABD7B9B6790F}">
-            <xm:f>ABS(D39-Solutions!$D$39)&lt;0.001</xm:f>
+          <x14:cfRule type="expression" priority="7" id="{320296C2-C020-41D7-AADE-55FB6C8E6AB3}">
+            <xm:f>NOT(ABS(D39-Solutions!D39)&lt;0.001)</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="8" id="{1096F20E-5F85-4D62-86B5-ABD7B9B6790F}">
+            <xm:f>ABS(D39-Solutions!D39)&lt;0.001</xm:f>
             <x14:dxf>
               <font>
                 <b/>
@@ -2158,40 +2440,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="3" id="{320296C2-C020-41D7-AADE-55FB6C8E6AB3}">
-            <xm:f>NOT(ABS(D39-Solutions!$D$39)&lt;0.001)</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i val="0"/>
-                <color rgb="FFFF0000"/>
-              </font>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D39</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{800A77BE-8BED-4697-8ABE-482CC82506CA}">
-            <xm:f>NOT(ABS(F39-Solutions!$D$39)&lt;0.001)</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i val="0"/>
-                <color rgb="FFFF0000"/>
-              </font>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{6ED09CE4-5C88-46C2-AC08-B0A6B78B95C4}">
-            <xm:f>ABS(F39-Solutions!$D$39)&lt;0.001</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i val="0"/>
-                <color rgb="FF00B050"/>
-              </font>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F39</xm:sqref>
+          <xm:sqref>D39:I39</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2203,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1BCCF5-0FED-40B4-A2E6-E7A0679B1D51}">
   <dimension ref="A11:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2259,10 +2508,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2608,20 +2857,24 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="31" t="s">
+      <c r="C30" s="44"/>
+      <c r="D30" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="31" t="s">
+      <c r="E30" s="44"/>
+      <c r="F30" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="52"/>
     </row>
     <row r="31" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
@@ -2645,25 +2898,35 @@
       <c r="G31" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="H31" s="46">
+        <v>13</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="28"/>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="32" t="s">
         <v>35</v>
       </c>
       <c r="E32" s="30"/>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="32" t="s">
         <v>35</v>
       </c>
       <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H32" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="48"/>
+    </row>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>36</v>
       </c>
@@ -2687,25 +2950,36 @@
       <c r="G33" s="18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="17">
+        <f>D14/A14</f>
+        <v>28.349523125000001</v>
+      </c>
+      <c r="I33" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="32" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="30"/>
-      <c r="F34" s="29" t="s">
+      <c r="F34" s="32" t="s">
         <v>35</v>
       </c>
       <c r="G34" s="30"/>
-    </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H34" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="48"/>
+    </row>
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>38</v>
       </c>
@@ -2729,28 +3003,39 @@
       <c r="G35" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="17">
+        <f>D21/A21</f>
+        <v>3.28084</v>
+      </c>
+      <c r="I35" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="29" t="s">
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="32" t="s">
         <v>35</v>
       </c>
       <c r="G36" s="30"/>
-    </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H36" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="48"/>
+    </row>
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="17">
         <f>D12/A12</f>
         <v>2.2046199999999998</v>
@@ -2758,25 +3043,36 @@
       <c r="G37" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="17">
+        <f>H35</f>
+        <v>3.28084</v>
+      </c>
+      <c r="I37" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="29" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="30"/>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="29" t="s">
         <v>2</v>
       </c>
       <c r="G38" s="30"/>
-    </row>
-    <row r="39" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="48"/>
+    </row>
+    <row r="39" spans="1:9" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
         <v>41</v>
       </c>
@@ -2800,15 +3096,30 @@
       <c r="G39" s="24" t="s">
         <v>34</v>
       </c>
+      <c r="H39" s="23">
+        <f>H31*H33*H35*H37</f>
+        <v>3966.9727084474698</v>
+      </c>
+      <c r="I39" s="50" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D3B99D0F-5290-4C19-9294-325A292E8E9A}" state="hidden" topLeftCell="A31">
-      <selection activeCell="G40" sqref="G40"/>
+    <customSheetView guid="{D3B99D0F-5290-4C19-9294-325A292E8E9A}" state="hidden" topLeftCell="A35">
+      <selection activeCell="I38" sqref="I38"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H30:I30"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:G38"/>
@@ -2818,13 +3129,6 @@
     <mergeCell ref="B36:C37"/>
     <mergeCell ref="D36:E37"/>
     <mergeCell ref="F36:G36"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>